<commit_message>
Buscando arquivo diretamente da pasta atual
</commit_message>
<xml_diff>
--- a/Dev Assistant.xlsx
+++ b/Dev Assistant.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\robertn\Downloads\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\robertn\Documents\Projetos\PYTHON\ai_sap_developer\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AD1C5248-7D17-4D14-B0F3-B18C4B2ABC6B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CEE3BE16-CB07-4096-AC63-B92A0B49D022}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{D222F31E-51F6-45E8-9DE9-D5A867BE515D}"/>
   </bookViews>
@@ -4495,10 +4495,20 @@
 exportar as informações na planilha "Mensagens.xlsm" a partir da segunda coluna</t>
   </si>
   <si>
+    <t>COHV
+variante /PS
+executar
+armazenar todos os dados da coluna "PROJN"
+CN47N
+colar todos os dados salvos no campo "Elemento PEP"
+escrever "/INI_MONT" no campo "Layout"
+executar
+escrever dados da tabela na planilha chamada "Esquema.xlsm"</t>
+  </si>
+  <si>
     <t># Default model for SAP automations, developed by Robert Aron Zimmermann, using Google AI Studio tuned prompt model
 from sap_functions import SAP
 from excel import ExcelHandler
-import progressbar
 default_language = 'PT'
 login = open('sap_login.txt', 'r').readline().strip().split(',')
 scheduled_execution = {'scheduled?': False, 'username': login[0], 'password': login[1], 'principal': '100'}
@@ -4534,17 +4544,6 @@
     work = Work()
     work.COHV()
     work.CN47N()</t>
-  </si>
-  <si>
-    <t>COHV
-variante /PS
-executar
-armazenar todos os dados da coluna "PROJN"
-CN47N
-colar todos os dados salvos no campo "Elemento PEP"
-escrever "/INI_MONT" no campo "Layout"
-executar
-escrever dados da tabela na planilha chamada "Esquema.xlsm"</t>
   </si>
 </sst>
 </file>
@@ -4949,14 +4948,14 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4AA211B0-CF30-4FF4-82D8-F1F44D488D73}">
   <dimension ref="A1:B85"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A84" workbookViewId="0">
-      <selection activeCell="A84" sqref="A84"/>
+    <sheetView tabSelected="1" topLeftCell="A80" workbookViewId="0">
+      <selection activeCell="A86" sqref="A86"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="111.85546875" style="1" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="85.85546875" style="1" customWidth="1"/>
+    <col min="2" max="2" width="113.7109375" style="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.25">
@@ -5183,7 +5182,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="29" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:2" ht="78.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A29" s="1" t="s">
         <v>53</v>
       </c>
@@ -5191,7 +5190,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="30" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:2" ht="78.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A30" s="1" t="s">
         <v>59</v>
       </c>
@@ -5199,7 +5198,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="31" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:2" ht="78.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A31" s="1" t="s">
         <v>58</v>
       </c>
@@ -5207,7 +5206,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="32" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:2" ht="78.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A32" s="1" t="s">
         <v>55</v>
       </c>
@@ -5215,7 +5214,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="33" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:2" ht="78.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A33" s="1" t="s">
         <v>73</v>
       </c>
@@ -5223,7 +5222,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="34" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:2" ht="78.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A34" s="1" t="s">
         <v>74</v>
       </c>
@@ -5231,7 +5230,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="35" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:2" ht="78.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A35" s="1" t="s">
         <v>61</v>
       </c>
@@ -5239,7 +5238,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="36" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:2" ht="78.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A36" s="1" t="s">
         <v>62</v>
       </c>
@@ -5247,7 +5246,7 @@
         <v>63</v>
       </c>
     </row>
-    <row r="37" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:2" ht="78.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A37" s="1" t="s">
         <v>66</v>
       </c>
@@ -5255,7 +5254,7 @@
         <v>65</v>
       </c>
     </row>
-    <row r="38" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:2" ht="78.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A38" s="1" t="s">
         <v>68</v>
       </c>
@@ -5263,7 +5262,7 @@
         <v>67</v>
       </c>
     </row>
-    <row r="39" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:2" ht="78.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A39" s="1" t="s">
         <v>69</v>
       </c>
@@ -5271,7 +5270,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="40" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:2" ht="78.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A40" s="1" t="s">
         <v>71</v>
       </c>
@@ -5279,7 +5278,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="41" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:2" ht="78.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A41" s="1" t="s">
         <v>75</v>
       </c>
@@ -5287,7 +5286,7 @@
         <v>76</v>
       </c>
     </row>
-    <row r="42" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:2" ht="78.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A42" s="1" t="s">
         <v>77</v>
       </c>
@@ -5295,7 +5294,7 @@
         <v>76</v>
       </c>
     </row>
-    <row r="43" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:2" ht="78.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A43" s="1" t="s">
         <v>79</v>
       </c>
@@ -5303,7 +5302,7 @@
         <v>78</v>
       </c>
     </row>
-    <row r="44" spans="1:2" ht="45" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:2" ht="78.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A44" s="2" t="s">
         <v>120</v>
       </c>
@@ -5311,7 +5310,7 @@
         <v>81</v>
       </c>
     </row>
-    <row r="45" spans="1:2" ht="120" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:2" ht="78.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A45" s="2" t="s">
         <v>121</v>
       </c>
@@ -5319,7 +5318,7 @@
         <v>82</v>
       </c>
     </row>
-    <row r="46" spans="1:2" ht="90" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:2" ht="78.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A46" s="2" t="s">
         <v>122</v>
       </c>
@@ -5327,7 +5326,7 @@
         <v>83</v>
       </c>
     </row>
-    <row r="47" spans="1:2" ht="135" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:2" ht="78.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A47" s="2" t="s">
         <v>108</v>
       </c>
@@ -5335,7 +5334,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="48" spans="1:2" ht="135" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:2" ht="78.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A48" s="2" t="s">
         <v>84</v>
       </c>
@@ -5343,7 +5342,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="49" spans="1:2" ht="105" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:2" ht="78.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A49" s="2" t="s">
         <v>123</v>
       </c>
@@ -5351,7 +5350,7 @@
         <v>88</v>
       </c>
     </row>
-    <row r="50" spans="1:2" ht="180" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:2" ht="78.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A50" s="2" t="s">
         <v>124</v>
       </c>
@@ -5359,7 +5358,7 @@
         <v>86</v>
       </c>
     </row>
-    <row r="51" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:2" ht="78.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A51" s="2" t="s">
         <v>89</v>
       </c>
@@ -5367,7 +5366,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="52" spans="1:2" ht="30" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:2" ht="78.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A52" s="1" t="s">
         <v>125</v>
       </c>
@@ -5375,7 +5374,7 @@
         <v>91</v>
       </c>
     </row>
-    <row r="53" spans="1:2" ht="30" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:2" ht="78.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A53" s="1" t="s">
         <v>126</v>
       </c>
@@ -5383,7 +5382,7 @@
         <v>87</v>
       </c>
     </row>
-    <row r="54" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:2" ht="78.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A54" s="1" t="s">
         <v>127</v>
       </c>
@@ -5391,7 +5390,7 @@
         <v>92</v>
       </c>
     </row>
-    <row r="55" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:2" ht="78.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A55" s="1" t="s">
         <v>128</v>
       </c>
@@ -5399,7 +5398,7 @@
         <v>93</v>
       </c>
     </row>
-    <row r="56" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:2" ht="78.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A56" s="1" t="s">
         <v>129</v>
       </c>
@@ -5407,7 +5406,7 @@
         <v>94</v>
       </c>
     </row>
-    <row r="57" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:2" ht="78.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A57" s="1" t="s">
         <v>130</v>
       </c>
@@ -5415,7 +5414,7 @@
         <v>95</v>
       </c>
     </row>
-    <row r="58" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:2" ht="78.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A58" s="1" t="s">
         <v>131</v>
       </c>
@@ -5423,7 +5422,7 @@
         <v>96</v>
       </c>
     </row>
-    <row r="59" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:2" ht="78.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A59" s="1" t="s">
         <v>132</v>
       </c>
@@ -5431,7 +5430,7 @@
         <v>97</v>
       </c>
     </row>
-    <row r="60" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:2" ht="78.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A60" s="1" t="s">
         <v>133</v>
       </c>
@@ -5439,7 +5438,7 @@
         <v>98</v>
       </c>
     </row>
-    <row r="61" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:2" ht="78.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A61" s="1" t="s">
         <v>119</v>
       </c>
@@ -5447,7 +5446,7 @@
         <v>99</v>
       </c>
     </row>
-    <row r="62" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:2" ht="78.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A62" s="1" t="s">
         <v>118</v>
       </c>
@@ -5455,7 +5454,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="63" spans="1:2" ht="30" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:2" ht="78.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A63" s="1" t="s">
         <v>117</v>
       </c>
@@ -5463,7 +5462,7 @@
         <v>101</v>
       </c>
     </row>
-    <row r="64" spans="1:2" ht="30" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:2" ht="78.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A64" s="1" t="s">
         <v>116</v>
       </c>
@@ -5471,7 +5470,7 @@
         <v>102</v>
       </c>
     </row>
-    <row r="65" spans="1:2" ht="30" x14ac:dyDescent="0.25">
+    <row r="65" spans="1:2" ht="78.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A65" s="1" t="s">
         <v>115</v>
       </c>
@@ -5479,7 +5478,7 @@
         <v>105</v>
       </c>
     </row>
-    <row r="66" spans="1:2" ht="30" x14ac:dyDescent="0.25">
+    <row r="66" spans="1:2" ht="78.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A66" s="1" t="s">
         <v>114</v>
       </c>
@@ -5487,7 +5486,7 @@
         <v>106</v>
       </c>
     </row>
-    <row r="67" spans="1:2" ht="30" x14ac:dyDescent="0.25">
+    <row r="67" spans="1:2" ht="78.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A67" s="1" t="s">
         <v>113</v>
       </c>
@@ -5495,7 +5494,7 @@
         <v>103</v>
       </c>
     </row>
-    <row r="68" spans="1:2" ht="30" x14ac:dyDescent="0.25">
+    <row r="68" spans="1:2" ht="78.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A68" s="1" t="s">
         <v>111</v>
       </c>
@@ -5503,7 +5502,7 @@
         <v>104</v>
       </c>
     </row>
-    <row r="69" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="69" spans="1:2" ht="78.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A69" s="1" t="s">
         <v>112</v>
       </c>
@@ -5511,7 +5510,7 @@
         <v>107</v>
       </c>
     </row>
-    <row r="70" spans="1:2" ht="120" x14ac:dyDescent="0.25">
+    <row r="70" spans="1:2" ht="78.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A70" s="2" t="s">
         <v>134</v>
       </c>
@@ -5519,7 +5518,7 @@
         <v>136</v>
       </c>
     </row>
-    <row r="71" spans="1:2" ht="165" x14ac:dyDescent="0.25">
+    <row r="71" spans="1:2" ht="78.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A71" s="2" t="s">
         <v>135</v>
       </c>
@@ -5527,7 +5526,7 @@
         <v>137</v>
       </c>
     </row>
-    <row r="72" spans="1:2" ht="90" x14ac:dyDescent="0.25">
+    <row r="72" spans="1:2" ht="78.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A72" s="2" t="s">
         <v>138</v>
       </c>
@@ -5535,7 +5534,7 @@
         <v>139</v>
       </c>
     </row>
-    <row r="73" spans="1:2" ht="105.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="73" spans="1:2" ht="78.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A73" s="2" t="s">
         <v>155</v>
       </c>
@@ -5543,7 +5542,7 @@
         <v>154</v>
       </c>
     </row>
-    <row r="74" spans="1:2" ht="153.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="74" spans="1:2" ht="78.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A74" s="2" t="s">
         <v>153</v>
       </c>
@@ -5551,7 +5550,7 @@
         <v>152</v>
       </c>
     </row>
-    <row r="75" spans="1:2" ht="67.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="75" spans="1:2" ht="78.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A75" s="2" t="s">
         <v>150</v>
       </c>
@@ -5559,7 +5558,7 @@
         <v>151</v>
       </c>
     </row>
-    <row r="76" spans="1:2" ht="132" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="76" spans="1:2" ht="78.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A76" s="2" t="s">
         <v>149</v>
       </c>
@@ -5567,7 +5566,7 @@
         <v>148</v>
       </c>
     </row>
-    <row r="77" spans="1:2" ht="109.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="77" spans="1:2" ht="78.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A77" s="2" t="s">
         <v>146</v>
       </c>
@@ -5575,7 +5574,7 @@
         <v>147</v>
       </c>
     </row>
-    <row r="78" spans="1:2" ht="67.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="78" spans="1:2" ht="78.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A78" s="2" t="s">
         <v>144</v>
       </c>
@@ -5583,7 +5582,7 @@
         <v>145</v>
       </c>
     </row>
-    <row r="79" spans="1:2" ht="90" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="79" spans="1:2" ht="78.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A79" s="2" t="s">
         <v>143</v>
       </c>
@@ -5591,7 +5590,7 @@
         <v>142</v>
       </c>
     </row>
-    <row r="80" spans="1:2" ht="79.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="80" spans="1:2" ht="78.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A80" s="2" t="s">
         <v>141</v>
       </c>
@@ -5599,7 +5598,7 @@
         <v>140</v>
       </c>
     </row>
-    <row r="81" spans="1:2" ht="186.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="81" spans="1:2" ht="78.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A81" s="2" t="s">
         <v>157</v>
       </c>
@@ -5607,7 +5606,7 @@
         <v>156</v>
       </c>
     </row>
-    <row r="82" spans="1:2" ht="105.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="82" spans="1:2" ht="78.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A82" s="2" t="s">
         <v>159</v>
       </c>
@@ -5615,7 +5614,7 @@
         <v>158</v>
       </c>
     </row>
-    <row r="83" spans="1:2" ht="234" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="83" spans="1:2" ht="78.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A83" s="2" t="s">
         <v>160</v>
       </c>
@@ -5623,7 +5622,7 @@
         <v>161</v>
       </c>
     </row>
-    <row r="84" spans="1:2" ht="162.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="84" spans="1:2" ht="78.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A84" s="2" t="s">
         <v>163</v>
       </c>
@@ -5631,12 +5630,12 @@
         <v>162</v>
       </c>
     </row>
-    <row r="85" spans="1:2" ht="95.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="85" spans="1:2" ht="78.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A85" s="2" t="s">
+        <v>164</v>
+      </c>
+      <c r="B85" s="2" t="s">
         <v>165</v>
-      </c>
-      <c r="B85" s="2" t="s">
-        <v>164</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Corrigindo problema na tradução ao alterar idioma
</commit_message>
<xml_diff>
--- a/Dev Assistant.xlsx
+++ b/Dev Assistant.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\robertn\Documents\Projetos\PYTHON\ai_sap_developer\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F4EB2E45-5EAB-40D7-845E-43C7B451BBD9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0D975DFE-E650-49AC-9E32-FD093AA5B332}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-28920" yWindow="-45" windowWidth="29040" windowHeight="15840" xr2:uid="{D222F31E-51F6-45E8-9DE9-D5A867BE515D}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{D222F31E-51F6-45E8-9DE9-D5A867BE515D}"/>
   </bookViews>
   <sheets>
     <sheet name="Inteligencia" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="170" uniqueCount="166">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="172" uniqueCount="168">
   <si>
     <t>Objetivo</t>
   </si>
@@ -4544,6 +4544,158 @@
     work = Work()
     work.COHV()
     work.ZTPP289()</t>
+  </si>
+  <si>
+    <t>Título: Verificação mensagens de exceção Usinagem
+Descrição: Automatização desenvolvida para realizar o verificar mensagens de exceção na Usinagem
+Solicitado por: Nicolas Gabriel Massaia Camacho
+Desenvolvido por: Robert Aron Zimmermann
+Observações:
+A planilha "Mensagens.xlsm" deve ser limpa no começo do procedimento
+Adicione tratativas de erro na MD04 para evitar que a execução seja interrompida
+Procedimento:
+Transação COHV
+Escrever Layout "/usin_exce"
+flegar "Ordens de produção"
+colar em "Centro de produção" os textos "1200" e "1220"
+No campo "Planejador MRP" escrever "200" e no até escrever "299"
+flegar "Com marcação/código eliminação"
+No campo "Data de liberação real" escrever "01.01.2023"
+No até de "Data de liberação real" escrever a data de hoje no formato "dd.mm.yyyy"
+executar
+Percorrer todas as linhas da tabela e salvar em uma lista chamada "materiais" todos os itens da coluna de id "MATNR" (não adicionar duplicatas)
+Acessar transação ZTPP289
+escrever no campo "Centro" o valor "1200"
+No campo "Planejador MRP" escrever "200" e no até escrever "299"
+no modo de seleção múltipla colar em "Centro" os textos "1200" e "1220"
+colar todos os itens da variável "materiais" no campo "Material"
+flegar o checkbox localizado na esquerda de cada um desses itens: "1 Antecipar", "2 Adiar, "3 Estornar" e "7 Excesso de estoque"
+executar
+Se a o número da janela atual for igual a 1, então clicar em "Sim"
+Dentro da tabela, inserir o Layout "/NICOLAS"
+exportar as informações na planilha "Mensagens.xlsm" a partir da segunda coluna
+A partir da segunda linha da segunda coluna na planilha "Mensagens.xlsm":
+pegar o "material" na coluna 6,
+acessar a transação MD04
+inserir no campo "Material" o valor "material"
+escrever no campo "Centro" o texto "1200"
+executar
+Percorrer a coluna 3 no campo Flex
+Ao encontrar "OrdPro" então clicar duas vezes no campo
+Armazenar o texto localizado 3 índices ao lado de "Exceção"
+pegar o texto que está entre a "/" e o ")"
+formatar esse texto em "dd/mm/yyyy"
+Escrever o texto na linha atual da planilha, coluna 9</t>
+  </si>
+  <si>
+    <t xml:space="preserve"># Default model for SAP automations, developed by Robert Aron Zimmermann, using Google AI Studio tuned prompt model;
+from sap_functions import SAP
+from excel import ExcelHandler
+import datetime
+import progressbar
+default_language = 'PT'
+login = open('sap_login.txt', 'r').readline().strip().split(',')
+scheduled_execution = {'scheduled?': False, 'username': login[0], 'password': login[1], 'principal': '100'}
+sap_window = 0
+# Verificação mensagens de exceção Usinagem
+# Automatização desenvolvida para realizar o verificar mensagens de exceção na Usinagem
+# Solicitado por Nicolas Gabriel Massaia Camacho
+# Desenvolvido por Robert Aron Zimmermann
+class Work:
+    def __init__(self):
+        self.sap = SAP(sap_window, scheduled_execution, default_language)
+        self.excel = ExcelHandler('Mensagens.xlsm')
+        self.materiais = []
+    def COHV(self):
+        self.sap.select_transaction('COHV')
+        self.sap.write_text_field('Layout','/usin_exce')
+        self.sap.flag_field('Ordens de produção', True)
+        self.sap.multiple_selection_field('Centro de produção')
+        self.sap.multiple_selection_paste_data('1200\n1220')
+        self.sap.write_text_field('Planejador MRP', '200')
+        self.sap.write_text_field_until('Planejador MRP', '299')
+        self.sap.flag_field('Com marcação/código eliminação', True)
+        self.sap.write_text_field('Data de liberação real', '01.01.2023')
+        self.sap.write_text_field_until('Data de liberação real', datetime.datetime.now().strftime('%d.%m.%Y'))
+        self.sap.run_actual_transaction()
+        my_grid = self.sap.get_my_grid()
+        rows = self.sap.get_my_grid_count_rows(my_grid)
+        for i in range(rows):
+            material = my_grid.getCellValue(i, 'MATNR')
+            if material not in self.materiais:
+                self.materiais.append(material)
+    def ZTPP289(self):
+        self.sap.select_transaction('ZTPP289')
+        self.sap.write_text_field('Centro','1200')
+        self.sap.write_text_field('Planejador MRP', '200')
+        self.sap.write_text_field_until('Planejador MRP', '299')
+        self.sap.multiple_selection_field('Centro')
+        self.sap.multiple_selection_paste_data('1200\n1220')
+        self.sap.multiple_selection_field('Material')
+        self.sap.multiple_selection_paste_data('\n'.join(self.materiais))
+        self.sap.flag_field_at_side('1 Antecipar', True, -1)
+        self.sap.flag_field_at_side('2 Adiar', True, -1)
+        self.sap.flag_field_at_side('3 Estornar', True, -1)
+        self.sap.flag_field_at_side('7 Excesso de estoque', True, -1)
+        self.sap.run_actual_transaction()
+        if self.sap.session.activeWindow.name == 'wnd[1]':
+            self.sap.press_button('Sim')
+        my_grid = self.sap.get_my_grid()
+        my_grid.pressToolbarContextButton("&amp;MB_VARIANT")
+        my_grid.selectContextMenuItem("&amp;LOAD")
+        layouts_grid = self.sap.get_my_grid()
+        layouts_grid.selectColumn('VARIANT')
+        layouts_grid.contextMenu()
+        layouts_grid.selectContextMenuItem('&amp;FILTER')
+        self.sap.write_text_field('Layout', '/NICOLAS')
+        self.sap.press_button('Executar')
+        layouts_grid.clickCurrentCell()
+        rows = self.sap.get_my_grid_count_rows(my_grid)
+        self.excel.load_workbook()
+        self.excel.select_sheet('Principal')
+        self.excel.clean_data(2, self.excel.count_columns(1), 2, self.excel.count_rows(2))
+        self.excel.sap_write_my_grid(my_grid, rows, 1, 2)
+        self.excel.save_workbook()
+        self.excel.close_workbook()
+    def MD04(self, mat):
+        try:
+            self.sap.select_transaction('MD04')
+            self.sap.write_text_field('Material', mat)
+            self.sap.write_text_field('Centro', '1200')
+            self.sap.run_actual_transaction()
+            my_table = self.sap.get_my_table()
+            table_rows = my_table.VisibleRowCount
+            for index in range(table_rows):
+                if self.sap.my_table_get_cell_value(my_table, index, 2) == 'OrdPro':
+                    my_table.getCell(index, 2).setFocus()
+                    self.sap.session.findById('wnd[0]').sendVKey(2)
+                    data = self.sap.get_text_at_side('Exceção', 3)
+                    indice_inicio = str(data).find('/') + 1
+                    indice_fim = str(data).find(')', indice_inicio)
+                    data_obj = datetime.datetime.strptime(data[indice_inicio:indice_fim], "%d.%m.%y")
+                    return data_obj.strftime("%d/%m/%Y")
+            return 'Not Found'
+        except Exception as e:
+            return f"Ocorreu o erro: {str(e)}"
+if __name__ == '__main__':
+    work = Work()
+    work.COHV()
+    work.ZTPP289()
+    excel = ExcelHandler('Mensagens.xlsm')
+    excel.load_workbook()
+    excel.select_sheet('Principal')
+    rows = excel.count_rows(2)
+    bar = progressbar.ProgressBar(rows - 1)
+    bar.start()
+    for i in range(2, rows + 1):
+        material = excel.get_cell(i, 6)
+        if material is not None:
+            msg = work.MD04(material)
+            excel.write_cell(i, 9, msg)
+            bar.update(i - 1)
+            excel.save_workbook()
+    excel.close_workbook()
+</t>
   </si>
 </sst>
 </file>
@@ -4946,10 +5098,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4AA211B0-CF30-4FF4-82D8-F1F44D488D73}">
-  <dimension ref="A1:B85"/>
+  <dimension ref="A1:B86"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A83" workbookViewId="0">
-      <selection activeCell="B86" sqref="B86"/>
+    <sheetView tabSelected="1" topLeftCell="A85" workbookViewId="0">
+      <selection activeCell="B90" sqref="B90"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -5638,6 +5790,14 @@
         <v>164</v>
       </c>
     </row>
+    <row r="86" spans="1:2" ht="128.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A86" s="2" t="s">
+        <v>166</v>
+      </c>
+      <c r="B86" s="2" t="s">
+        <v>167</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
Criando novo script de envio de E-mail
</commit_message>
<xml_diff>
--- a/Dev Assistant.xlsx
+++ b/Dev Assistant.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\robertn\Documents\Projetos\PYTHON\ai_sap_developer\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0D975DFE-E650-49AC-9E32-FD093AA5B332}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B1F5E375-657C-4FFF-AB51-7AC8325428CD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{D222F31E-51F6-45E8-9DE9-D5A867BE515D}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="172" uniqueCount="168">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="174" uniqueCount="170">
   <si>
     <t>Objetivo</t>
   </si>
@@ -3536,62 +3536,6 @@
 caso o título da janela atual seja "Seleciona um local para impressão" então selecionar a option "Visualizar Docto no spool" e pressionar o botão "Avançar"
 Se o título da janela atual for "Informação" então pressionar no botão "Avançar"
 Clicar em "Gravar"</t>
-  </si>
-  <si>
-    <t># Default model for SAP automations, developed by Robert Aron Zimmermann, using Google AI Studio tuned prompt model
-from sap_functions import SAP
-from excel import ExcelHandler
-from outlook import Outlook
-default_language = 'EN'
-login = open('sap_login.txt', 'r').readline().strip().split(',')
-scheduled_execution = {'scheduled?': False, 'username': login[0], 'password': login[1], 'principal': '100'}
-sap_window = 0
-# Production Order Release 
-# To start Production, orders need to be released using COHV transaction  and before that
-# Workflow Must be clear. to track the Work Flow Using ZTMM069.
-# Solicitado por Selvaganapathy S
-# Desenvolvido por Robert Aron Zimmermann
-class Work:
-    def __init__(self):
-        self.sap = SAP(sap_window, scheduled_execution, default_language)
-        self.materials = []
-        self.users = []
-        self.excel = ExcelHandler('Orders.xlsm')
-    def COHV(self):
-        self.sap.select_transaction('COHV')
-        self.sap.insert_variant('SARANYAM')
-        self.sap.run_actual_transaction()
-        my_grid = self.sap.get_my_grid()
-        rows = self.sap.get_my_grid_count_rows(my_grid)
-        for i in range(rows):
-            self.materials.append(my_grid.getCellValue(i, 'MATNR'))
-    def ZTMM069(self):
-        self.sap.select_transaction('ZTMM069')
-        self.sap.clean_all_fields()
-        self.sap.write_text_field('Interval of days', '999')
-        self.sap.write_text_field('Plant', '6200')
-        self.sap.write_text_field('Layout', '/RAJBLOCK')
-        self.sap.multiple_selection_field('Material')
-        self.sap.multiple_selection_paste_data('\n'.join(self.materials))
-        self.sap.run_actual_transaction()
-        my_grid = self.sap.get_my_grid()
-        rows = self.sap.get_my_grid_count_rows(my_grid)
-        for i in range(rows):
-            if f"{my_grid.getCellValue(i, 'USER')}@weg.net" not in self.users:
-                self.users.append(f"{my_grid.getCellValue(i, 'USER')}@weg.net")
-        self.excel.load_workbook()
-        self.excel.select_sheet('Principal')
-        self.excel.clean_data(2, self.excel.count_columns(1), 2, self.excel.count_rows(2))
-        self.excel.sap_write_my_grid(my_grid, rows, 1, 2)
-        self.excel.save_workbook()
-        self.excel.close_workbook()
-if __name__ == '__main__':
-    mail_outlook = Outlook()
-    work = Work()
-    work.COHV()
-    work.ZTMM069()
-    mail_outlook.send_email('Production Order Release', ';'.join(work.users),
-                            'The Production Order Release spreadsheet follows...', attachments=f'Orders.xlsm')</t>
   </si>
   <si>
     <t>Título: Impressão de Ordens
@@ -4696,6 +4640,213 @@
             excel.save_workbook()
     excel.close_workbook()
 </t>
+  </si>
+  <si>
+    <t># Default model for SAP automations, developed by Robert Aron Zimmermann, using Google AI Studio tuned prompt model
+from sap_functions import SAP
+from outlook import Outlook
+import progressbar
+default_language = 'PT'
+login = open('sap_login.txt', 'r').readline().strip().split(',')
+scheduled_execution = {'scheduled?': False, 'username': login[0], 'password': login[1], 'principal': '100'}
+sap_window = 0
+# Cobrança de materiais WMO para GTA
+# Automatização desenvolvida para efetuar a cobrança de matérias brutos utilizados na fabricação de peças usinadas
+# para alternadores, dos metalúrgicos e usinagem de eixos da WMO.
+# Solicitado por Beatriz Silva de Andrade Graciosa
+# Desenvolvido por Robert Aron Zimmermann
+def read_file(filename):
+    clients = []
+    with open(filename, 'r') as file:
+        lines = file.readlines()
+        for line in lines:
+            data = line.strip().split(',')
+            clients.append({'mrp': data[0], 'name': data[1], 'email': data[2]})
+    return clients
+def get_copy(filename):
+    with open(filename, 'r') as file:
+        lines = file.readlines()
+        for line in lines:
+            return line
+class Work:
+    def __init__(self):
+        self.sap = SAP(sap_window, scheduled_execution, default_language)
+        self.orders = ''
+        self.materials = []
+        self.results = []
+        self.clients = read_file('clients.txt')
+        self.copy = get_copy('copy_email.txt')
+    def COOIS(self):
+        self.sap.select_transaction('COOIS')
+        self.sap.insert_variant('MATERIAIS GTA')
+        self.sap.run_actual_transaction()
+        my_grid = self.sap.get_my_grid()
+        row_number = self.sap.get_my_grid_count_rows(my_grid)
+        for i in range(row_number):
+            self.orders = f"{self.orders}{my_grid.getCellValue(i, 'AUFNR')}\n"
+    def CO24(self):
+        self.sap.select_transaction('CO24')
+        self.sap.write_text_field('Layout', '/LISTA_MAT')
+        self.sap.multiple_selection_field('Ordem')
+        self.sap.multiple_selection_paste_data(self.orders)
+        self.sap.run_actual_transaction()
+        my_grid = self.sap.get_my_grid()
+        row_number = self.sap.get_my_grid_count_rows(my_grid)
+        for i in range(row_number):
+            if my_grid.getCellValue(i, 'MATNR') not in self.materials:
+                self.materials.append(my_grid.getCellValue(i, 'MATNR'))
+    def MD04(self, material):
+        self.sap.select_transaction('MD04')
+        self.sap.write_text_field('Material', material)
+        self.sap.write_text_field('Centro', '1200')
+        self.sap.run_actual_transaction()
+        my_table = self.sap.get_my_table()
+        target_column = my_table.getCell(-1, 7).Text
+        if target_column == 'Centro fornec./recept.':
+            for i in range(my_table.VisibleRowCount):
+                center = my_table.getCell(i, 7).Text
+                if center != '':
+                    self.sap.write_text_field('Centro', str(center))
+                    self.sap.run_actual_transaction()
+                    my_table = self.sap.get_my_table()
+                    for i2 in range(my_table.VisibleRowCount):
+                        qty_available = my_table.getCell(0, 5).Text
+                        if int(qty_available) &gt; 0:
+                            self.sap.press_button('Expandir detalh.cabeç.')
+                            plan_mrp = self.sap.get_text_at_side('Planejador MRP', 1)
+                            return self.results.append(
+                                {'material': material, 'quantity': qty_available, 'center': center,
+                                 'mrp': str(plan_mrp)})
+                        else:
+                            return
+if __name__ == '__main__':
+    work = Work()
+    email = Outlook()
+    work.COOIS()
+    work.CO24()
+    bar = progressbar.ProgressBar(max_value=len(work.materials) - 1)
+    for index in range(len(work.materials)):
+        work.MD04(str(work.materials[index]))
+        bar.update(index)
+    texto_email = {}
+    for item in work.clients:
+        texto_email[item['name']] = ''
+    for result in work.results:
+        nome_area = next((item['name'] for item in work.clients if item['mrp'] == result['mrp']), None)
+        email_area = next((item['email'] for item in work.clients if item['mrp'] == result['mrp']), None)
+        if nome_area is not None and email_area is not None:
+            texto_email[
+                nome_area] = f"{texto_email[nome_area]}{result['material']} possui disponível {result['quantity']} no centro {result['center']}&lt;br&gt;"
+        else:
+            print(f"O planejador {result['mrp']} não está sendo cobrado! Insira o mesmo no arquivo de texto!")
+    body_mail = ''
+    receptores = ''
+    for item in work.clients:
+        if texto_email[item['name']] != '':
+            receptores = f"{receptores}{item['email']};"
+            body_mail = f"{body_mail}&lt;h4&gt;{item['name']}&lt;/h4&gt;&lt;h5&gt;{texto_email[item['name']]}&lt;/h5&gt;&lt;br&gt;"
+    email.send_email('Materiais WEN', receptores,
+                     f"Bom dia,&lt;br&gt;&lt;br&gt;Gentileza enviar pedido abaixo com o lote completo, materiais já se "
+                     f"encontram em estoque&lt;br&gt;&lt;br&gt;{body_mail}",
+                     work.copy)</t>
+  </si>
+  <si>
+    <t>Título: Cobrança de materiais WMO para GTA
+Descrição: Automatização desenvolvida para efetuar a cobrança de matérias brutos utilizados na fabricação de peças usinadas para alternadores, dos metalúrgicos e usinagem de eixos da WMO.
+Solicitado por: Beatriz Silva de Andrade Graciosa
+Desenvolvido por: Robert Aron Zimmermann
+Acessar a transação COOIS
+Inserir variante "MATERIAIS GTA"
+executar
+percorrer tabela inserindo os dados da coluna "AUFNR" em uma variável de texto chamada orders
+Criar um dicionário chamado "clients", adicionar dados de um arquivo chamado "clients.txt" separando por virgulas, nesse arquivo existe os campos "mrp","name" e "email"
+Criar uma string chamada "copy", percorrer todas as lnhas de um arquivo chamado "copy_email.txt" e ler todas as linhas do mesmo
+Acessar transação CO24
+no campo "Layout" escrever "/LISTA_MAT"
+colar a variável "orders" na seleção múltipla do campo "Ordem"
+executar
+Percorrer as linhas da tabela verificando se o item do campo "MATNR" não está na lista materials
+Se não estiver dentro da lista então acrescentar na mesma
+Para cada item de "work.materials":
+Acessar transação MD04
+inserir no campo "Material" o respectivo material
+Inserir no campo "Centro" o texto "1200"
+executar transação
+Caso o título da coluna 7 do campo Flex seja igual a "Centro fornec./recept.":
+Percorrer as linhas visíveis do campo Flex:
+armazenar o valor da célula em uma variável chamada "center"
+Caso "center" seja diferente de vazio então:
+Escrever no campo "Centro" o valor de "center" convertido em texto
+executar
+Armazenar em uma variável chamada qty_avaiable o valor da linha 0 da coluna 5 do campo Flex convertido em inteiro
+Caso qty_avaiable seja maior que 0:
+Pressionar o botão "Expandir detalh.cabeç."
+armazenar em uma variável chamada "plan_mrp" o texto ao lado de "Planejador MRP"
+Armazenar em um dicionário o respectivo material, a variável "qty_avaiable", a variável "center" e "plan_mrp"
+Caso não seja maior que 0 então retornar
+Para cada item do dicionário criado anteriormente realizar o procedimento abaixo:
+coletar o nome da área e email da área fazendo relação do campo "mrp" entre os dicionários "clients" e "results"
+caso encontre os dois campos então adicionar o texto em um dicionário chamado "texto_email": "{nome da área}{número material} possui disponível {quantidade} no centro {número do centro}"
+Caso não encontre então fazer um print avisando que o respectivo "mrp" não está sendo cobrado
+Enviar um email com todos os "email" de "clients", em cópia adicionar a string "copy", o título dele deve ser "Materiais WEN", o corpo do email deve seguir o modelo:
+Bom dia,
+Gentileza enviar abaixo com o lote completo, materiais já se encontram em estoque
+{Percorrer todo o dicionário "texto_email" e  escrever:} {nome do cliente}{texto_email}</t>
+  </si>
+  <si>
+    <t># Default model for SAP automations, developed by Robert Aron Zimmermann, using Google AI Studio tuned prompt model
+from sap_functions import SAP
+from excel import ExcelHandler
+default_language = 'EN'
+login = open('sap_login.txt', 'r').readline().strip().split(',')
+scheduled_execution = {'scheduled?': False, 'username': login[0], 'password': login[1], 'principal': '100'}
+sap_window = 0
+# Production Order Release 
+# To start Production, orders need to be released using COHV transaction  and before that
+# Workflow Must be clear. to track the Work Flow Using ZTMM069.
+# Solicitado por Selvaganapathy S
+# Desenvolvido por Robert Aron Zimmermann
+class Work:
+    def __init__(self):
+        self.sap = SAP(sap_window, scheduled_execution, default_language)
+        self.materials = []
+        self.users = []
+        self.excel = ExcelHandler('Orders.xlsm')
+    def COHV(self):
+        self.sap.select_transaction('COHV')
+        self.sap.insert_variant('SARANYAM')
+        self.sap.run_actual_transaction()
+        my_grid = self.sap.get_my_grid()
+        rows = self.sap.get_my_grid_count_rows(my_grid)
+        for i in range(rows):
+            self.materials.append(my_grid.getCellValue(i, 'MATNR'))
+    def ZTMM069(self):
+        self.sap.select_transaction('ZTMM069')
+        self.sap.clean_all_fields()
+        self.sap.write_text_field('Interval of days', '999')
+        self.sap.write_text_field('Plant', '6200')
+        self.sap.write_text_field('Layout', '/RAJBLOCK')
+        self.sap.multiple_selection_field('Material')
+        self.sap.multiple_selection_paste_data('\n'.join(self.materials))
+        self.sap.run_actual_transaction()
+        my_grid = self.sap.get_my_grid()
+        rows = self.sap.get_my_grid_count_rows(my_grid)
+        for i in range(rows):
+            if f"{my_grid.getCellValue(i, 'USER')}@weg.net" not in self.users:
+                self.users.append(f"{my_grid.getCellValue(i, 'USER')}@weg.net")
+        self.excel.load_workbook()
+        self.excel.select_sheet('Principal')
+        self.excel.clean_data(2, self.excel.count_columns(1), 2, self.excel.count_rows(2))
+        self.excel.sap_write_my_grid(my_grid, rows, 1, 2)
+        self.excel.save_workbook()
+        self.excel.close_workbook()
+if __name__ == '__main__':
+    mail_outlook = Outlook()
+    work = Work()
+    work.COHV()
+    work.ZTMM069()
+    mail_outlook.send_email('Production Order Release', ';'.join(work.users),
+                            'The Production Order Release spreadsheet follows...', attachments=f'Orders.xlsm')</t>
   </si>
 </sst>
 </file>
@@ -5098,10 +5249,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4AA211B0-CF30-4FF4-82D8-F1F44D488D73}">
-  <dimension ref="A1:B86"/>
+  <dimension ref="A1:B87"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A85" workbookViewId="0">
-      <selection activeCell="B90" sqref="B90"/>
+    <sheetView tabSelected="1" topLeftCell="A83" workbookViewId="0">
+      <selection activeCell="B87" sqref="B87"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -5688,42 +5839,42 @@
     </row>
     <row r="73" spans="1:2" ht="78.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A73" s="2" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="B73" s="2" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
     </row>
     <row r="74" spans="1:2" ht="78.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A74" s="2" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="B74" s="2" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
     </row>
     <row r="75" spans="1:2" ht="78.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A75" s="2" t="s">
+        <v>149</v>
+      </c>
+      <c r="B75" s="2" t="s">
         <v>150</v>
-      </c>
-      <c r="B75" s="2" t="s">
-        <v>151</v>
       </c>
     </row>
     <row r="76" spans="1:2" ht="78.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A76" s="2" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="B76" s="2" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
     </row>
     <row r="77" spans="1:2" ht="78.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A77" s="2" t="s">
+        <v>145</v>
+      </c>
+      <c r="B77" s="2" t="s">
         <v>146</v>
-      </c>
-      <c r="B77" s="2" t="s">
-        <v>147</v>
       </c>
     </row>
     <row r="78" spans="1:2" ht="78.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -5731,7 +5882,7 @@
         <v>144</v>
       </c>
       <c r="B78" s="2" t="s">
-        <v>145</v>
+        <v>169</v>
       </c>
     </row>
     <row r="79" spans="1:2" ht="78.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -5752,49 +5903,57 @@
     </row>
     <row r="81" spans="1:2" ht="78.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A81" s="2" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="B81" s="2" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
     </row>
     <row r="82" spans="1:2" ht="78.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A82" s="2" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="B82" s="2" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
     </row>
     <row r="83" spans="1:2" ht="78.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A83" s="2" t="s">
+        <v>159</v>
+      </c>
+      <c r="B83" s="2" t="s">
         <v>160</v>
-      </c>
-      <c r="B83" s="2" t="s">
-        <v>161</v>
       </c>
     </row>
     <row r="84" spans="1:2" ht="78.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A84" s="2" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="B84" s="2" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
     </row>
     <row r="85" spans="1:2" ht="78.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A85" s="2" t="s">
+        <v>162</v>
+      </c>
+      <c r="B85" s="2" t="s">
         <v>163</v>
-      </c>
-      <c r="B85" s="2" t="s">
-        <v>164</v>
       </c>
     </row>
     <row r="86" spans="1:2" ht="128.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A86" s="2" t="s">
+        <v>165</v>
+      </c>
+      <c r="B86" s="2" t="s">
         <v>166</v>
       </c>
-      <c r="B86" s="2" t="s">
+    </row>
+    <row r="87" spans="1:2" ht="91.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A87" s="2" t="s">
+        <v>168</v>
+      </c>
+      <c r="B87" s="2" t="s">
         <v>167</v>
       </c>
     </row>

</xml_diff>